<commit_message>
Update Risultati App non ottimizzata.xlsx
</commit_message>
<xml_diff>
--- a/RisultatiPowDroid/Risultati App non ottimizzata.xlsx
+++ b/RisultatiPowDroid/Risultati App non ottimizzata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biagi\Desktop\Progetto-Operating_systems_for_mobile_cloud_and_IoT\RisultatiPowDroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C257D8-0D03-4731-AFD4-0274D9B30A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E54C46C-398D-4507-906F-ADEF40E2C0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risultati App non ottimizzata" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,12 +148,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -161,6 +155,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,42 +263,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -301,10 +304,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -358,16 +361,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Scenario5:</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Energy (J)</a:t>
+              <a:rPr lang="en-GB"/>
+              <a:t>Scenario5</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -410,17 +405,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Risultati App non ottimizzata'!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Energy (J)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -443,6 +427,30 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Risultati App non ottimizzata'!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>102.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.717</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.81399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Risultati App non ottimizzata'!$D$5:$D$9</c:f>
@@ -470,7 +478,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-730C-4668-9974-39D8D40D8F1F}"/>
+              <c16:uniqueId val="{00000000-9752-4391-86FA-63FAB127AE8E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -482,11 +490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1100902688"/>
-        <c:axId val="1303990240"/>
+        <c:axId val="1902193055"/>
+        <c:axId val="1893190431"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1100902688"/>
+        <c:axId val="1902193055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,7 +535,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Prova</a:t>
+                  <a:t>Duration (S)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -561,6 +569,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -597,12 +606,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1303990240"/>
+        <c:crossAx val="1893190431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1303990240"/>
+        <c:axId val="1893190431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +652,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Joule</a:t>
+                  <a:t>Energy (J)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -714,7 +723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100902688"/>
+        <c:crossAx val="1902193055"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -790,27 +799,13 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
+            <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:sysClr>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -818,15 +813,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Scenario3: Energy (J)</a:t>
+              <a:rPr lang="en-GB"/>
+              <a:t>Scenario3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -843,27 +831,13 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
+          <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -883,19 +857,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Risultati App non ottimizzata'!$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Energy (J)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -916,6 +879,30 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Risultati App non ottimizzata'!$H$5:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40.329000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.984000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.356000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.929000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39.134999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Risultati App non ottimizzata'!$I$5:$I$9</c:f>
@@ -943,7 +930,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6A9D-493D-B6B7-80BAE2E6EF41}"/>
+              <c16:uniqueId val="{00000000-7C04-4109-82FD-AC656B87A90A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -955,11 +942,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1100902688"/>
-        <c:axId val="1303990240"/>
+        <c:axId val="1836171807"/>
+        <c:axId val="2058411871"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1100902688"/>
+        <c:axId val="1836171807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,8 +987,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Prova</a:t>
+                  <a:t>Duration</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (S)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1034,6 +1026,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1070,12 +1063,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1303990240"/>
+        <c:crossAx val="2058411871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1303990240"/>
+        <c:axId val="2058411871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1109,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Joule</a:t>
+                  <a:t>Energy (J)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1187,7 +1180,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100902688"/>
+        <c:crossAx val="1836171807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1277,15 +1270,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Scenario2: Energy (J)</a:t>
+              <a:rPr lang="en-GB"/>
+              <a:t>Scenario2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1328,19 +1314,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Risultati App non ottimizzata'!$N$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Energy (J)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1361,6 +1336,30 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Risultati App non ottimizzata'!$M$5:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>138.566</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.81700000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139.88499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137.89099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Risultati App non ottimizzata'!$N$5:$N$9</c:f>
@@ -1388,7 +1387,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0479-4FCD-B109-A91197A68A22}"/>
+              <c16:uniqueId val="{00000000-AF2B-4C86-A743-98339F195FE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1400,11 +1399,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1100902688"/>
-        <c:axId val="1303990240"/>
+        <c:axId val="2067421727"/>
+        <c:axId val="2058406415"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1100902688"/>
+        <c:axId val="2067421727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,8 +1444,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Prova</a:t>
+                  <a:t>Duration</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (S)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1479,6 +1483,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1515,12 +1520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1303990240"/>
+        <c:crossAx val="2058406415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1303990240"/>
+        <c:axId val="2058406415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1566,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Joule</a:t>
+                  <a:t>Energy (J)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1632,7 +1637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100902688"/>
+        <c:crossAx val="2067421727"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1703,38 +1708,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>APP: Energy (J)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1773,19 +1746,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Risultati App non ottimizzata'!$S$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Energy (J)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1806,6 +1768,24 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Risultati App non ottimizzata'!$R$5:$R$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>138.95179999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.946600000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.67720000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Risultati App non ottimizzata'!$S$5:$S$7</c:f>
@@ -1827,7 +1807,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-03A8-4050-B2E2-3F2993ECB1A7}"/>
+              <c16:uniqueId val="{00000000-140F-435D-9831-59AFC25430A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1839,11 +1819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1100902688"/>
-        <c:axId val="1303990240"/>
+        <c:axId val="1836169887"/>
+        <c:axId val="2058383599"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1100902688"/>
+        <c:axId val="1836169887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1884,7 +1864,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Scenario</a:t>
+                  <a:t>Duration (S)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1918,6 +1898,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1954,12 +1935,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1303990240"/>
+        <c:crossAx val="2058383599"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1303990240"/>
+        <c:axId val="2058383599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +1981,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Joule</a:t>
+                  <a:t>Energy (J)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2071,7 +2052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1100902688"/>
+        <c:crossAx val="1836169887"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4356,22 +4337,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>22523</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>358140</xdr:rowOff>
+      <xdr:rowOff>354106</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>169545</xdr:rowOff>
+      <xdr:colOff>18602</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65548D95-E273-51AB-7C79-EED56C86BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948CD649-88EE-8ECE-8C27-BCD5FA7F9D46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4392,28 +4373,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>15241</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>12439</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1102995</xdr:colOff>
+      <xdr:colOff>1088877</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>173355</xdr:rowOff>
+      <xdr:rowOff>347383</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF52BFE1-B2BB-4736-8EBB-7F67CA1F479E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9210984E-B078-1950-74B7-28522FFAE95D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4430,28 +4409,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>18602</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1102995</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>169545</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCB44DEC-1AEA-4E23-890E-8209DC5F0A18}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C27F77F-CF05-E083-CAF8-B3F9E412E923}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4467,29 +4444,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>5715</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1092462</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>10533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>46729</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>150495</xdr:rowOff>
+      <xdr:rowOff>347383</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40CE539-1C0A-4600-91A5-CC0F79C66E37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAE8C3E2-54FD-CF38-AD05-777E1A0B63A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4771,528 +4746,508 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H9" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
-    <col min="2" max="5" width="16.21875" style="1"/>
-    <col min="6" max="6" width="9.109375" style="1" customWidth="1"/>
-    <col min="7" max="10" width="16.21875" style="1"/>
-    <col min="11" max="11" width="9.109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="16.21875" style="1"/>
+    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="2" max="5" width="16.21875" style="2"/>
+    <col min="6" max="6" width="9.109375" style="2" customWidth="1"/>
+    <col min="7" max="10" width="16.21875" style="2"/>
+    <col min="11" max="11" width="9.109375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="16.21875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="G4" s="6" t="s">
+      <c r="E4" s="4"/>
+      <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="L4" s="6" t="s">
+      <c r="J4" s="4"/>
+      <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="8"/>
-      <c r="Q4" s="6" t="s">
+      <c r="O4" s="4"/>
+      <c r="Q4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="8"/>
+      <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>102.97</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>107.099188</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="G5" s="9" t="s">
+      <c r="E5" s="5"/>
+      <c r="G5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>40.329000000000001</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>82.498931999999996</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="L5" s="9" t="s">
+      <c r="J5" s="5"/>
+      <c r="L5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>138.566</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>192.95286899999999</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="Q5" s="9" t="s">
+      <c r="O5" s="5"/>
+      <c r="Q5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="6">
         <f>M12</f>
         <v>138.95179999999999</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="6">
         <f>N12</f>
         <v>180.15037240000001</v>
       </c>
-      <c r="T5" s="10"/>
+      <c r="T5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>101.68</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>79.198443999999995</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="G6" s="9" t="s">
+      <c r="E6" s="5"/>
+      <c r="G6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>39.984000000000002</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>41.610183999999997</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="L6" s="9" t="s">
+      <c r="J6" s="5"/>
+      <c r="L6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <v>138.81700000000001</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>205.80058399999999</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="Q6" s="9" t="s">
+      <c r="O6" s="5"/>
+      <c r="Q6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="6">
         <f>H12</f>
         <v>39.946600000000004</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="6">
         <f>I12</f>
         <v>54.237206999999998</v>
       </c>
-      <c r="T6" s="10"/>
+      <c r="T6" s="5"/>
     </row>
     <row r="7" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>106.717</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>150.24098000000001</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="G7" s="9" t="s">
+      <c r="E7" s="5"/>
+      <c r="G7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>40.356000000000002</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>35.400556999999999</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="L7" s="9" t="s">
+      <c r="J7" s="5"/>
+      <c r="L7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>139.88499999999999</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>199.97241500000001</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="Q7" s="9" t="s">
+      <c r="O7" s="5"/>
+      <c r="Q7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="6">
         <f>C12</f>
         <v>103.67720000000001</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="6">
         <f>D12</f>
         <v>114.88823659999998</v>
       </c>
-      <c r="T7" s="10"/>
+      <c r="T7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>103.81399999999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>146.27462</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="G8" s="9" t="s">
+      <c r="E8" s="5"/>
+      <c r="G8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>39.929000000000002</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>35.813851999999997</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="L8" s="9" t="s">
+      <c r="J8" s="5"/>
+      <c r="L8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <v>139.6</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>150.84999300000001</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="10"/>
+      <c r="O8" s="5"/>
+      <c r="Q8" s="7"/>
+      <c r="T8" s="5"/>
     </row>
     <row r="9" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>103.205</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>91.627950999999996</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="G9" s="9" t="s">
+      <c r="E9" s="5"/>
+      <c r="G9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>39.134999999999998</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>75.86251</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="L9" s="9" t="s">
+      <c r="J9" s="5"/>
+      <c r="L9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>137.89099999999999</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>151.17600100000001</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="5" t="s">
+      <c r="O9" s="5"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="S9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="10"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="10"/>
-      <c r="Q10" s="13" t="s">
+      <c r="B10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="G10" s="7"/>
+      <c r="J10" s="5"/>
+      <c r="L10" s="7"/>
+      <c r="O10" s="5"/>
+      <c r="Q10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="6">
         <f>AVERAGE(R5:R7)</f>
         <v>94.19186666666667</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="6">
         <f>AVERAGE(S5:S7)</f>
         <v>116.42527199999999</v>
       </c>
-      <c r="T10" s="10">
+      <c r="T10" s="5">
         <f t="shared" ref="T10:T11" si="0">S10/R10</f>
         <v>1.236043791466779</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="5" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="O11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="13" t="s">
+      <c r="Q11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="6">
         <f>MEDIAN(R5:R7)</f>
         <v>103.67720000000001</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="6">
         <f>MEDIAN(S5:S7)</f>
         <v>114.88823659999998</v>
       </c>
-      <c r="T11" s="10">
+      <c r="T11" s="5">
         <f t="shared" si="0"/>
         <v>1.1081340603334191</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="6">
         <f>AVERAGE(C5:C9)</f>
         <v>103.67720000000001</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="6">
         <f>AVERAGE(D5:D9)</f>
         <v>114.88823659999998</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="5">
         <f>D12/C12</f>
         <v>1.1081340603334191</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="6">
         <f>AVERAGE(H5:H9)</f>
         <v>39.946600000000004</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="6">
         <f t="shared" ref="I12" si="1">AVERAGE(I5:I9)</f>
         <v>54.237206999999998</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="5">
         <f t="shared" ref="J12:J13" si="2">I12/H12</f>
         <v>1.3577427615867181</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="6">
         <f t="shared" ref="M12:N12" si="3">AVERAGE(M5:M9)</f>
         <v>138.95179999999999</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="6">
         <f t="shared" si="3"/>
         <v>180.15037240000001</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="5">
         <f t="shared" ref="O12:O13" si="4">N12/M12</f>
         <v>1.2964954207142334</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="8">
         <f>_xlfn.STDEV.P(R5:R7)</f>
         <v>40.971421487774741</v>
       </c>
-      <c r="S12" s="15">
+      <c r="S12" s="8">
         <f>_xlfn.STDEV.P(S5:S7)</f>
         <v>51.415323031353083</v>
       </c>
-      <c r="T12" s="16" t="s">
+      <c r="T12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="6">
         <f>MEDIAN(C5:C9)</f>
         <v>103.205</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="6">
         <f>MEDIAN(D5:D9)</f>
         <v>107.099188</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="5">
         <f>D13/C13</f>
         <v>1.0377325517174556</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="6">
         <f t="shared" ref="H13:I13" si="5">MEDIAN(H5:H9)</f>
         <v>39.984000000000002</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="6">
         <f t="shared" si="5"/>
         <v>41.610183999999997</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="5">
         <f t="shared" si="2"/>
         <v>1.0406708683473389</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="6">
         <f t="shared" ref="M13:N13" si="6">MEDIAN(M5:M9)</f>
         <v>138.81700000000001</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="6">
         <f t="shared" si="6"/>
         <v>192.95286899999999</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="5">
         <f t="shared" si="4"/>
         <v>1.3899801105051974</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="8">
         <f>_xlfn.STDEV.P(C5:C9)</f>
         <v>1.6715867192580807</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="8">
         <f>_xlfn.STDEV.P(D5:D9)</f>
         <v>28.67191304728658</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="8">
         <f t="shared" ref="H14" si="7">_xlfn.STDEV.P(H5:H9)</f>
         <v>0.44141617550787721</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="8">
         <f>_xlfn.STDEV.P(I5:I9)</f>
         <v>20.591551337082336</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="8">
         <f t="shared" ref="M14:N14" si="8">_xlfn.STDEV.P(M5:M9)</f>
         <v>0.71879549247334473</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="8">
         <f t="shared" si="8"/>
         <v>24.136184777893302</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="9" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>